<commit_message>
Documentation and presentation links Added
</commit_message>
<xml_diff>
--- a/Project Documents/IC-Agile-Project-Charter-11390.xlsx
+++ b/Project Documents/IC-Agile-Project-Charter-11390.xlsx
@@ -1,32 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newma\Bank Software Project\bank_apps\Project Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD831F8-A049-40A6-BB95-56C757D54B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Project Charter" sheetId="1" r:id="rId1"/>
-    <sheet name="- Disclaimer -" sheetId="3" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="LEADS_table">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Project Charter'!$B$2:$E$16</definedName>
-    <definedName name="Type" localSheetId="1">'[1]Maintenance Work Order'!#REF!</definedName>
     <definedName name="Type">#REF!</definedName>
     <definedName name="valHighlight">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -46,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>GENERAL PROJECT INFORMATION</t>
   </si>
@@ -75,12 +64,6 @@
     <t>EXPECTED START DATE</t>
   </si>
   <si>
-    <t xml:space="preserve">Any articles, templates, or information provided by Smartsheet on the website are for reference only. While we strive to keep the information up to date and correct, we make no representations or warranties of any kind, express or implied, about the completeness, accuracy, reliability, suitability, or availability with respect to the website or the information, articles, templates, or related graphics contained on the website. Any reliance you place on such information is therefore strictly at your own risk. </t>
-  </si>
-  <si>
-    <t>CLICK HERE TO CREATE IN SMARTSHEET</t>
-  </si>
-  <si>
     <t>VISION</t>
   </si>
   <si>
@@ -94,9 +77,6 @@
   </si>
   <si>
     <t>AGILE PROJECT CHARTER TEMPLATE</t>
-  </si>
-  <si>
-    <t>Supreme Bank of Britain (SBOB)</t>
   </si>
   <si>
     <t>Mark Ugbelase</t>
@@ -127,16 +107,19 @@
   </si>
   <si>
     <t>Rohit</t>
+  </si>
+  <si>
+    <t>Online Banking Application</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,20 +142,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -220,14 +189,8 @@
       <name val="Century Gothic"/>
       <family val="1"/>
     </font>
-    <font>
-      <u/>
-      <sz val="22"/>
-      <color theme="0"/>
-      <name val="Century Gothic Bold"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,12 +207,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00BD32"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -277,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -327,15 +284,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -472,12 +420,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -485,132 +432,121 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{1DBACFF4-FB77-E743-92B1-CF1651F1F286}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -652,7 +588,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3826E738-DEBF-114F-BAA6-A6B8EB745560}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3826E738-DEBF-114F-BAA6-A6B8EB745560}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -679,23 +615,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Maintenance Work Order"/>
-      <sheetName val="BLANK - Maintenance Work Order "/>
-      <sheetName val="- Disclaimer -"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1019,19 +938,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD54"/>
+  <dimension ref="A1:AD53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="3.296875" style="2" customWidth="1"/>
     <col min="2" max="2" width="13.796875" style="2" customWidth="1"/>
@@ -1041,53 +960,53 @@
     <col min="7" max="16384" width="10.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" customFormat="1" ht="196.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-    </row>
-    <row r="2" spans="1:30" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-    </row>
-    <row r="3" spans="1:30" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
+    <row r="1" spans="1:30" customFormat="1" ht="196.95" customHeight="1">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:30" customFormat="1" ht="42" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+    </row>
+    <row r="3" spans="1:30" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1097,13 +1016,13 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26" t="s">
+    <row r="4" spans="1:30" ht="21" customHeight="1" thickTop="1">
+      <c r="B4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1113,13 +1032,13 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="31"/>
+    <row r="5" spans="1:30" ht="34.950000000000003" customHeight="1">
+      <c r="B5" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1129,15 +1048,15 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="32" t="s">
+    <row r="6" spans="1:30" ht="19.95" customHeight="1">
+      <c r="B6" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="37"/>
+      <c r="D6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="1"/>
@@ -1149,16 +1068,16 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>17</v>
+    <row r="7" spans="1:30" ht="34.950000000000003" customHeight="1">
+      <c r="B7" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1169,13 +1088,13 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="32" t="s">
+    <row r="8" spans="1:30" ht="19.95" customHeight="1">
+      <c r="B8" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1185,13 +1104,13 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
+    <row r="9" spans="1:30" ht="34.950000000000003" customHeight="1">
+      <c r="B9" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1201,16 +1120,16 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="38" t="s">
+    <row r="10" spans="1:30" ht="19.95" customHeight="1">
+      <c r="B10" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>13</v>
+      <c r="C10" s="35"/>
+      <c r="D10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1221,15 +1140,15 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:30" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="17">
+    <row r="11" spans="1:30" ht="34.950000000000003" customHeight="1">
+      <c r="B11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="14">
         <v>45343</v>
       </c>
       <c r="F11" s="1"/>
@@ -1241,7 +1160,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:30" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="10.050000000000001" customHeight="1">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1255,13 +1174,13 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:30" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="1:30" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1271,15 +1190,15 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:30" ht="145.05000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
+    <row r="14" spans="1:30" ht="145.05000000000001" customHeight="1" thickTop="1">
+      <c r="B14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1289,15 +1208,15 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:30" ht="145.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
+    <row r="15" spans="1:30" ht="145.05000000000001" customHeight="1">
+      <c r="B15" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
+      <c r="C15" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1307,15 +1226,15 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:30" ht="145.05000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24"/>
+    <row r="16" spans="1:30" ht="145.05000000000001" customHeight="1" thickBot="1">
+      <c r="B16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1325,7 +1244,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="2:13" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" ht="10.050000000000001" customHeight="1">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1339,15 +1258,21 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="2:13" s="8" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="2:13">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1361,7 +1286,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1375,7 +1300,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1389,7 +1314,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1403,7 +1328,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1417,7 +1342,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1431,7 +1356,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1445,7 +1370,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1459,7 +1384,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1473,7 +1398,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1487,7 +1412,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1501,7 +1426,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1515,7 +1440,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1529,7 +1454,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1543,7 +1468,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:13">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1557,7 +1482,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1571,7 +1496,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1585,7 +1510,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:13">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1599,7 +1524,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:13">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1613,7 +1538,7 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1627,7 +1552,7 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1641,7 +1566,7 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1655,7 +1580,7 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:13">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1669,7 +1594,7 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:13">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1683,7 +1608,7 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:13">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1697,7 +1622,7 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:13">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1711,7 +1636,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:13">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1725,7 +1650,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:13">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1739,7 +1664,7 @@
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1753,7 +1678,7 @@
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:13">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1767,7 +1692,7 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:13">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1781,7 +1706,7 @@
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:13">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1795,7 +1720,7 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:13">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1809,7 +1734,7 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:13">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1823,7 +1748,7 @@
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:13">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1837,25 +1762,10 @@
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C16:E16"/>
-    <mergeCell ref="B18:E18"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B8:E8"/>
@@ -1867,46 +1777,13 @@
     <mergeCell ref="C14:E14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B18:E18" r:id="rId1" display="CLICK HERE TO CREATE IN SMARTSHEET" xr:uid="{C53907D5-1CEC-E841-B6AA-A76BF9C7550A}"/>
-  </hyperlinks>
   <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.4" header="0" footer="0"/>
   <pageSetup scale="99" fitToHeight="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4309677-E78B-7B46-8442-00A10BB8BE0F}">
-  <sheetPr>
-    <tabColor theme="1" tint="0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="B1:B2"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Y95" sqref="Y95"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3.296875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="88.296875" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:2" ht="105" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>